<commit_message>
Corrección de errores - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_003.xlsx
+++ b/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\02_Evaluacion_Desarrollador\Rechazadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0782E025-9005-400B-B7CA-6088FDC84DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F52B05-F469-4834-A70D-E4FC21F257B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26CA7BAA-0F1D-4022-BA09-5EA660A58557}"/>
   </bookViews>
@@ -92,12 +92,6 @@
     <t>No aplicable, ya que la propuesta ha sido rechazada. Sin embargo, si se hubiera considerado, el tiempo estimado podría haber sido de 4-6 semanas, dada la complejidad de integración y pruebas en múltiples dispositivos y sistemas operativos.</t>
   </si>
   <si>
-    <t xml:space="preserve"> La necesidad de colaborar estrechamente con proveedores de servicios de notificaciones y posiblemente el desarrollo de componentes adicionales para gestionar la programación de recordatorios en diferentes plataformas.</t>
-  </si>
-  <si>
-    <t>Los principales riesgos identificados incluyen la variabilidad en la entrega de notificaciones entre diferentes dispositivos y sistemas operativos, lo que podría resultar en una experiencia de usuario inconsistente. Además, la gestión de permisos de usuario y la privacidad de los datos son aspectos críticos que incrementan la complejidad de esta funcionalidad.</t>
-  </si>
-  <si>
     <t>Nicolás Barcia Quintela</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>EvalDes_003</t>
+  </si>
+  <si>
+    <t>No aplicable, ya que la propuesta ha sido rechazada. Sin embargo, si se hubiera considerado, la necesidad de trabajar con librerías externas compatibles con distintos sistemas operativos y dispositivos, para tener una experiencia de usuario uniforme.</t>
+  </si>
+  <si>
+    <t>Los principales riesgos identificados incluyen la variabilidad en la entrega de notificaciones entre diferentes dispositivos y sistemas operativos, lo que podría resultar en una experiencia de usuario inconsistente, además de depender de librerías externas. La gestión de permisos de usuario y la privacidad de los datos son aspectos críticos que incrementan la complejidad de esta funcionalidad.</t>
   </si>
 </sst>
 </file>
@@ -523,38 +523,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -568,71 +577,62 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2908033D-BFA4-47F7-BB8A-F564B2EAC35D}">
   <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -977,24 +977,24 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="40"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
@@ -1007,12 +1007,12 @@
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
+      <c r="F7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
@@ -1021,12 +1021,12 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="F8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
@@ -1035,12 +1035,12 @@
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="F9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1055,10 +1055,10 @@
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="40"/>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
@@ -1071,13 +1071,13 @@
         <v>8</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="45"/>
+      <c r="F13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
@@ -1094,35 +1094,35 @@
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" s="10"/>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C17" s="10"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C18" s="10"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="44"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C19" s="10"/>
@@ -1138,15 +1138,15 @@
     </row>
     <row r="21" spans="3:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="10"/>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C22" s="10"/>
@@ -1162,35 +1162,35 @@
     </row>
     <row r="24" spans="3:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
-      <c r="D24" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="47"/>
+      <c r="D24" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C25" s="10"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="50"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C26" s="10"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="53"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C27" s="10"/>
@@ -1206,46 +1206,46 @@
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C29" s="10"/>
-      <c r="D29" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="41"/>
+      <c r="D29" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="51"/>
       <c r="P29" s="15"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C30" s="10"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="54"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C31" s="10"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="54"/>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C32" s="10"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="44"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="57"/>
     </row>
     <row r="33" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="16"/>
@@ -1258,30 +1258,21 @@
       <c r="J33" s="18"/>
     </row>
     <row r="34" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23" t="s">
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="D24:J26"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
     <mergeCell ref="C34:H34"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="C9:E9"/>
@@ -1295,6 +1286,15 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="D29:J32"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="D24:J26"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{6115D836-35A4-40A7-B824-FFCA3AD5F4C0}"/>

</xml_diff>

<commit_message>
Información actualizada - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_003.xlsx
+++ b/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\02_Evaluacion_Desarrollador\Rechazadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0782E025-9005-400B-B7CA-6088FDC84DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F52B05-F469-4834-A70D-E4FC21F257B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26CA7BAA-0F1D-4022-BA09-5EA660A58557}"/>
   </bookViews>
@@ -92,12 +92,6 @@
     <t>No aplicable, ya que la propuesta ha sido rechazada. Sin embargo, si se hubiera considerado, el tiempo estimado podría haber sido de 4-6 semanas, dada la complejidad de integración y pruebas en múltiples dispositivos y sistemas operativos.</t>
   </si>
   <si>
-    <t xml:space="preserve"> La necesidad de colaborar estrechamente con proveedores de servicios de notificaciones y posiblemente el desarrollo de componentes adicionales para gestionar la programación de recordatorios en diferentes plataformas.</t>
-  </si>
-  <si>
-    <t>Los principales riesgos identificados incluyen la variabilidad en la entrega de notificaciones entre diferentes dispositivos y sistemas operativos, lo que podría resultar en una experiencia de usuario inconsistente. Además, la gestión de permisos de usuario y la privacidad de los datos son aspectos críticos que incrementan la complejidad de esta funcionalidad.</t>
-  </si>
-  <si>
     <t>Nicolás Barcia Quintela</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>EvalDes_003</t>
+  </si>
+  <si>
+    <t>No aplicable, ya que la propuesta ha sido rechazada. Sin embargo, si se hubiera considerado, la necesidad de trabajar con librerías externas compatibles con distintos sistemas operativos y dispositivos, para tener una experiencia de usuario uniforme.</t>
+  </si>
+  <si>
+    <t>Los principales riesgos identificados incluyen la variabilidad en la entrega de notificaciones entre diferentes dispositivos y sistemas operativos, lo que podría resultar en una experiencia de usuario inconsistente, además de depender de librerías externas. La gestión de permisos de usuario y la privacidad de los datos son aspectos críticos que incrementan la complejidad de esta funcionalidad.</t>
   </si>
 </sst>
 </file>
@@ -523,38 +523,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -568,71 +577,62 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2908033D-BFA4-47F7-BB8A-F564B2EAC35D}">
   <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -977,24 +977,24 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="40"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
@@ -1007,12 +1007,12 @@
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
+      <c r="F7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
@@ -1021,12 +1021,12 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="F8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
@@ -1035,12 +1035,12 @@
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="F9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1055,10 +1055,10 @@
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="40"/>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
@@ -1071,13 +1071,13 @@
         <v>8</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="45"/>
+      <c r="F13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
@@ -1094,35 +1094,35 @@
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" s="10"/>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C17" s="10"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C18" s="10"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="44"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C19" s="10"/>
@@ -1138,15 +1138,15 @@
     </row>
     <row r="21" spans="3:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="10"/>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C22" s="10"/>
@@ -1162,35 +1162,35 @@
     </row>
     <row r="24" spans="3:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
-      <c r="D24" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="47"/>
+      <c r="D24" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C25" s="10"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="50"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C26" s="10"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="53"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C27" s="10"/>
@@ -1206,46 +1206,46 @@
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C29" s="10"/>
-      <c r="D29" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="41"/>
+      <c r="D29" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="51"/>
       <c r="P29" s="15"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C30" s="10"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="54"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C31" s="10"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="54"/>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C32" s="10"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="44"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="57"/>
     </row>
     <row r="33" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="16"/>
@@ -1258,30 +1258,21 @@
       <c r="J33" s="18"/>
     </row>
     <row r="34" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23" t="s">
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="D24:J26"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
     <mergeCell ref="C34:H34"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="C9:E9"/>
@@ -1295,6 +1286,15 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="D29:J32"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="D24:J26"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{6115D836-35A4-40A7-B824-FFCA3AD5F4C0}"/>

</xml_diff>